<commit_message>
actualizacion criterios de limpieza
</commit_message>
<xml_diff>
--- a/mercado_libre/API/criterios_de_limpieza.xlsx
+++ b/mercado_libre/API/criterios_de_limpieza.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Dropbox\TESIS_2021\mercado_libre\API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Dropbox\TFG\mercado_libre\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Apartamentos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Apartamentos!$A$1:$J$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Apartamentos!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="154">
   <si>
     <t xml:space="preserve"> id </t>
   </si>
@@ -482,10 +482,13 @@
     <t>Zona en la que se ubica el apartamento respecto a la calle Avenida Italia en continuación con la calle 18 de Julio (Norte o Sur).</t>
   </si>
   <si>
-    <t>Se calcula el percentil 75% de precio entre los apartamentos que cumplan con la condición price &lt; 40.000 y se eliminan observaciones con precio inferiror a dicho percentil. Se eliminan todas las observaciones que contengan una secuencia de 3 o más números repetidos en la variable price (i.e. 11111, 5555, etc.). Se pasan todos los importes a dólares estadounidenses utilizando el valor del tipo de cambio actual (web scrapping a página del INE: https://www.ine.gub.uy/).</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Se separa el valor numérico de la moneda en la que está expresado: maintenance_fee = valor numérico, maintenance_fee_unidad = moneda. Se pasan todos los importes a dólares estadounidenses utilizando el valor del tipo de cambio actual (web scrapping a página del INE: https://www.ine.gub.uy/). Se topea valores en UYU 50.000, se considera que valores superiores son datos incorrectos y se asigna NA.</t>
+  </si>
+  <si>
+    <t>Se calcula el percentil 75% de precio entre los apartamentos que cumplan con la condición price &lt; 40.000 y se eliminan observaciones con precio inferior a dicho percentil. Se eliminan todas las observaciones que contengan una secuencia de 3 o más números repetidos en la variable price (i.e. 11111, 5555, etc.). Se pasan todos los importes a dólares estadounidenses utilizando el valor del tipo de cambio actual (web scrapping a página del INE: https://www.ine.gub.uy/).</t>
+  </si>
+  <si>
+    <t>Si title contiene la palabra edificio y no contiene la palabra apartamento y ademas el precio es superior a USD 1.000.000 se considera que no se trata de un apartamento a la venta sino que se trata de un edificio a la venta y se elimina la observación.</t>
   </si>
 </sst>
 </file>
@@ -825,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,7 +894,7 @@
         <v>59</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -905,7 +908,7 @@
         <v>60</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1579,7 +1582,7 @@
         <v>121</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>124</v>
@@ -1713,6 +1716,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
actualizamos criterios de limpieza total area y covered area
</commit_message>
<xml_diff>
--- a/mercado_libre/API/criterios_de_limpieza.xlsx
+++ b/mercado_libre/API/criterios_de_limpieza.xlsx
@@ -426,21 +426,12 @@
     <t>Se considera que valores superiores a 10 son datos incorrectos y se les asigna NA. Se recodifica la variable a 1 para los casos en que vale 0 ó 1 (valor 0 se considera dato incorrecto y se le asigna 1), 2 o más en otro caso.</t>
   </si>
   <si>
-    <t>Se separa el valor numérico de la unidad de medida: covered_area = valor numérico, covered_area_unidad = unidad de medida. Se eliminan todas las observaciones que contengan una secuencia de 3 o más números repetidos  (i.e. 11111, 5555, etc.)</t>
-  </si>
-  <si>
-    <t>Se separa el valor numérico de la unidad de medida: total_area = valor numérico, total_area_unidad = unidad de medida. Se eliminan todas las observaciones que contengan una secuencia de 3 o más números repetidos  (i.e. 11111, 5555, etc.)</t>
-  </si>
-  <si>
     <t>no_covered_area</t>
   </si>
   <si>
     <t>Área no cubierta.</t>
   </si>
   <si>
-    <t>Se calcula como la diferencia entre total_area y covered_area. Cuando toma valor negativo se considera que los daots son incorrectos y se asigna NA.</t>
-  </si>
-  <si>
     <t>Se utiliza para el caso que haya que realizar conversiones a dólares estadounidenses y luego se elimina.</t>
   </si>
   <si>
@@ -541,6 +532,15 @@
   </si>
   <si>
     <t>Lo malo: hay datos que estaban correctos pero que por encontrarse sobre avd italia - 18 cuando se uso el baricentro del barrio quedo en zonas diferente (ej  sur cuando en realidad era norte)</t>
+  </si>
+  <si>
+    <t>Se separa el valor numérico de la unidad de medida: covered_area = valor numérico, covered_area_unidad = unidad de medida. Se eliminan todas las observaciones que contengan una secuencia de 3 o más números repetidos  (i.e. 11111, 5555, etc.). Adicionalmente para valores demasiado grandes, se decide tomar cómo dato erróneo todo valor superior a 1000 y se le imputa NA.</t>
+  </si>
+  <si>
+    <t>Se calcula como la diferencia entre total_area y covered_area. Cuando toma valor negativo se considera que los daots son incorrectos y se asigna NA. Adicionalmente para valores demasiado grandes, se decide tomar cómo dato erróneo todo valor superior a 1000 y se le imputa NA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se separa el valor numérico de la unidad de medida: total_area = valor numérico, total_area_unidad = unidad de medida. Se eliminan todas las observaciones que contengan una secuencia de 3 o más números repetidos  (i.e. 11111, 5555, etc.). Adicionalmente para valores demasiado grandes, se decide tomar cómo dato erróneo todo valor superior a 1000 y se le imputa NA.  </t>
   </si>
 </sst>
 </file>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +918,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>54</v>
@@ -952,7 +952,7 @@
         <v>59</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -966,7 +966,7 @@
         <v>60</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -980,7 +980,7 @@
         <v>61</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1078,7 +1078,7 @@
         <v>70</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1092,7 +1092,7 @@
         <v>71</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1232,7 +1232,7 @@
         <v>81</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1246,7 +1246,7 @@
         <v>82</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,7 +1274,7 @@
         <v>113</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="J27" t="s">
         <v>13</v>
@@ -1285,7 +1285,7 @@
         <v>112</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>119</v>
@@ -1342,7 +1342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>116</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="J32" t="s">
         <v>20</v>
@@ -1364,7 +1364,7 @@
         <v>115</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>117</v>
@@ -1401,7 +1401,7 @@
         <v>88</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J35" t="s">
         <v>23</v>
@@ -1486,7 +1486,7 @@
         <v>93</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>94</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1514,7 +1514,7 @@
         <v>95</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
         <v>96</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>97</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1556,7 +1556,7 @@
         <v>98</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1570,7 +1570,7 @@
         <v>99</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
         <v>100</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1598,7 +1598,7 @@
         <v>101</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,7 @@
         <v>102</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1626,7 +1626,7 @@
         <v>103</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1640,7 +1640,7 @@
         <v>121</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>124</v>
@@ -1651,7 +1651,7 @@
         <v>120</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>123</v>
@@ -1671,7 +1671,7 @@
         <v>104</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E53" s="2"/>
     </row>
@@ -1708,13 +1708,13 @@
         <v>125</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1722,7 +1722,7 @@
         <v>128</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>129</v>
@@ -1731,57 +1731,57 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="D59" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="C60" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1803,73 +1803,73 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizamos eda, criterios de limpieza y auxiliar informe
</commit_message>
<xml_diff>
--- a/mercado_libre/API/criterios_de_limpieza.xlsx
+++ b/mercado_libre/API/criterios_de_limpieza.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="174">
   <si>
     <t xml:space="preserve"> id </t>
   </si>
@@ -541,6 +541,15 @@
   </si>
   <si>
     <t xml:space="preserve">Se separa el valor numérico de la unidad de medida: total_area = valor numérico, total_area_unidad = unidad de medida. Se eliminan todas las observaciones que contengan una secuencia de 3 o más números repetidos  (i.e. 11111, 5555, etc.). Adicionalmente para valores demasiado grandes, se decide tomar cómo dato erróneo todo valor superior a 1000 y se le imputa NA.  </t>
+  </si>
+  <si>
+    <t>ingresomedio_ECH</t>
+  </si>
+  <si>
+    <t>Ingreso medio por barrio según datos de la Encuesta Contínua de Hogares 2021.</t>
+  </si>
+  <si>
+    <t>Se calcula el ingreso medio por barrio de los hogares en base a información de la ECH. La variable utilizada para construirlos es HT11: INGRESO TOTAL DEL HOGAR CON VALOR LOCATIVO SIN SERVICIO DOMÉSTICO (medido en pesos uruguayos). Se realiza una recodificación Bajo, Medio-Bajo, Medio-Alto, y Alto utilizando los cuartiles.</t>
   </si>
 </sst>
 </file>
@@ -884,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1773,7 +1782,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>149</v>
       </c>
@@ -1782,6 +1791,20 @@
       </c>
       <c r="C61" s="4" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>